<commit_message>
Added test with MLP 2 layers of 100 neurones
</commit_message>
<xml_diff>
--- a/Performances.xlsx
+++ b/Performances.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Walid\UniCode\CSI4506\CSI4506-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B4D9842-8555-4369-88ED-67F73A6D9228}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{901E6B32-7689-48A6-AA99-F2EE50E71FCE}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{19EFBD5C-037A-4BF2-AE76-DE1F99D575BF}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
   <si>
     <t>MAE</t>
   </si>
@@ -58,6 +58,11 @@
   </si>
   <si>
     <t>1 layer
+100 neurones
+5 epochs</t>
+  </si>
+  <si>
+    <t>2 layers 
 100 neurones
 5 epochs</t>
   </si>
@@ -439,10 +444,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92BAAC9C-E2D3-4E2D-BBD1-EB8D077F2CFC}">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -535,20 +540,32 @@
         <v>68.594705249537199</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
+      <c r="B5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="5">
+        <v>5.2778660554429901</v>
+      </c>
+      <c r="D5" s="5">
+        <v>45.036594244948503</v>
+      </c>
+      <c r="E5" s="5">
+        <v>5.4288098774124496</v>
+      </c>
+      <c r="F5" s="5">
+        <v>46.7165688643625</v>
+      </c>
+      <c r="G5" s="5">
+        <v>6.3103776719362301</v>
+      </c>
+      <c r="H5" s="5">
+        <v>67.626021486366</v>
+      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
-        <v>7</v>
-      </c>
+      <c r="A6" s="3"/>
       <c r="B6" s="2"/>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -558,7 +575,9 @@
       <c r="H6" s="5"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="3"/>
+      <c r="A7" s="3" t="s">
+        <v>7</v>
+      </c>
       <c r="B7" s="2"/>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
@@ -567,14 +586,24 @@
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
     </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="3"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+    </row>
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="A7:A8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
GridCVSearch for MLP full feature
</commit_message>
<xml_diff>
--- a/Performances.xlsx
+++ b/Performances.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Walid\UniCode\CSI4506\CSI4506-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD0226F7-0308-48F7-9FFF-4CE93122F6BD}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E36E952-95A7-4933-9D28-EC2A6555A6AD}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{19EFBD5C-037A-4BF2-AE76-DE1F99D575BF}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
   <si>
     <t>MAE</t>
   </si>
@@ -91,6 +91,19 @@
 1 layer
 75 neurones
 15 epoch</t>
+  </si>
+  <si>
+    <t>Optimizer</t>
+  </si>
+  <si>
+    <t>Not optimzed</t>
+  </si>
+  <si>
+    <t>{'activation': 'relu',
+ 'alpha': 0.0001,
+ 'hidden_layer_sizes': (100,),
+ 'max_iter': 100,
+ 'solver': 'adam'}</t>
   </si>
 </sst>
 </file>
@@ -473,7 +486,7 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -686,11 +699,17 @@
         <v>67.626021486366</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A10" s="4"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
+      <c r="B10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="3">
+        <v>5.27602081386918</v>
+      </c>
+      <c r="D10" s="3">
+        <v>45.204771334127301</v>
+      </c>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
@@ -700,9 +719,15 @@
       <c r="A11" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="1"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
+      <c r="B11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="3">
+        <v>5.3455557041292696</v>
+      </c>
+      <c r="D11" s="3">
+        <v>46.244431329590597</v>
+      </c>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
@@ -710,13 +735,27 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="4"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
+      <c r="B12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="3">
+        <v>5.4270249068444798</v>
+      </c>
+      <c r="D12" s="3">
+        <v>65.779687929005604</v>
+      </c>
+      <c r="E12" s="3">
+        <v>5.5168872981630397</v>
+      </c>
+      <c r="F12" s="3">
+        <v>67.335938575919002</v>
+      </c>
+      <c r="G12" s="3">
+        <v>7.0065944302804404</v>
+      </c>
+      <c r="H12" s="3">
+        <v>114.065545082369</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>

<commit_message>
GridCVSearch for lw and full feature sets
</commit_message>
<xml_diff>
--- a/Performances.xlsx
+++ b/Performances.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Walid\UniCode\CSI4506\CSI4506-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E36E952-95A7-4933-9D28-EC2A6555A6AD}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44311243-D4F0-4042-907D-3E8DEDF0C88E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{19EFBD5C-037A-4BF2-AE76-DE1F99D575BF}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="19">
   <si>
     <t>MAE</t>
   </si>
@@ -104,6 +104,12 @@
  'hidden_layer_sizes': (100,),
  'max_iter': 100,
  'solver': 'adam'}</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>{'activation': 'relu', 'alpha': 0.0001, 'hidden_layer_sizes': (100, 50, 10), 'max_iter': 200, 'solver': 'adam'}</t>
   </si>
 </sst>
 </file>
@@ -483,9 +489,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92BAAC9C-E2D3-4E2D-BBD1-EB8D077F2CFC}">
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
@@ -699,72 +705,104 @@
         <v>67.626021486366</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="A10" s="4"/>
       <c r="B10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="3">
+        <v>5.2500945110751598</v>
+      </c>
+      <c r="F10" s="3">
+        <v>44.559833252168097</v>
+      </c>
+      <c r="G10" s="3">
+        <v>6.39620928808767</v>
+      </c>
+      <c r="H10" s="3">
+        <v>67.998787696666597</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A11" s="4"/>
+      <c r="B11" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C11" s="3">
         <v>5.27602081386918</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D11" s="3">
         <v>45.204771334127301</v>
       </c>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="4" t="s">
+      <c r="E11" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B12" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C12" s="3">
         <v>5.3455557041292696</v>
       </c>
-      <c r="D11" s="3">
+      <c r="D12" s="3">
         <v>46.244431329590597</v>
       </c>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="4"/>
-      <c r="B12" s="1" t="s">
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" s="4"/>
+      <c r="B13" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C13" s="3">
         <v>5.4270249068444798</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D13" s="3">
         <v>65.779687929005604</v>
       </c>
-      <c r="E12" s="3">
+      <c r="E13" s="3">
         <v>5.5168872981630397</v>
       </c>
-      <c r="F12" s="3">
+      <c r="F13" s="3">
         <v>67.335938575919002</v>
       </c>
-      <c r="G12" s="3">
+      <c r="G13" s="3">
         <v>7.0065944302804404</v>
       </c>
-      <c r="H12" s="3">
+      <c r="H13" s="3">
         <v>114.065545082369</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="A12:A13"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:A10"/>
+    <mergeCell ref="A4:A11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>